<commit_message>
add Excel format testst, catch fatal errors
</commit_message>
<xml_diff>
--- a/inst/extdata/incorrect_formats.xlsx
+++ b/inst/extdata/incorrect_formats.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726843FA-02BE-49E3-833E-AE980E210F6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDE8E69-25AF-4848-838E-944932A7D99F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20820" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sylvia" sheetId="6" r:id="rId1"/>
-    <sheet name="Sheet1 (5)" sheetId="5" state="hidden" r:id="rId2"/>
-    <sheet name="Sheet1 (4)" sheetId="4" state="hidden" r:id="rId3"/>
-    <sheet name="Sheet1 (3)" sheetId="3" state="hidden" r:id="rId4"/>
-    <sheet name="Sheet1 (2)" sheetId="2" state="hidden" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId6"/>
+    <sheet name="format-01" sheetId="6" r:id="rId1"/>
+    <sheet name="format-02" sheetId="8" r:id="rId2"/>
+    <sheet name="format-03" sheetId="9" r:id="rId3"/>
+    <sheet name="format-04" sheetId="11" r:id="rId4"/>
+    <sheet name="format-empty" sheetId="10" r:id="rId5"/>
+    <sheet name="Sheet1 (5)" sheetId="5" state="hidden" r:id="rId6"/>
+    <sheet name="Sheet1 (4)" sheetId="4" state="hidden" r:id="rId7"/>
+    <sheet name="Sheet1 (3)" sheetId="3" state="hidden" r:id="rId8"/>
+    <sheet name="Sheet1 (2)" sheetId="2" state="hidden" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="81">
   <si>
     <t>Con 1</t>
   </si>
@@ -247,6 +251,27 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>What</t>
+  </si>
+  <si>
+    <t>This is a grid with some notes and some more errors</t>
+  </si>
+  <si>
+    <t>Some</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random </t>
+  </si>
+  <si>
+    <t xml:space="preserve">text </t>
+  </si>
+  <si>
+    <t xml:space="preserve">and </t>
+  </si>
+  <si>
+    <t>numbers</t>
   </si>
 </sst>
 </file>
@@ -352,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -397,6 +422,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,17 +714,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B74F4B3-50A5-4152-AB10-43E3FD8B1294}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="A1:J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" customWidth="1"/>
+    <col min="1" max="1" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="12">
         <v>999</v>
       </c>
@@ -722,7 +756,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -754,7 +788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>27</v>
       </c>
@@ -786,7 +820,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>68</v>
       </c>
@@ -818,7 +852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>28</v>
       </c>
@@ -850,7 +884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>67</v>
       </c>
@@ -882,7 +916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>29</v>
       </c>
@@ -914,7 +948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>66</v>
       </c>
@@ -946,7 +980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>31</v>
       </c>
@@ -978,7 +1012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>32</v>
       </c>
@@ -1010,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>33</v>
       </c>
@@ -1042,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>65</v>
       </c>
@@ -1074,7 +1108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>35</v>
       </c>
@@ -1106,7 +1140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>36</v>
       </c>
@@ -1138,7 +1172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>69</v>
       </c>
@@ -1170,7 +1204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>37</v>
       </c>
@@ -1202,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>70</v>
       </c>
@@ -1234,7 +1268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
         <v>38</v>
       </c>
@@ -1266,10 +1300,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I20" s="7"/>
     </row>
   </sheetData>
@@ -1278,7 +1312,1417 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401460AA-074C-4CB5-A831-402A114BB149}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="12">
+        <v>999</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="12">
+        <v>1</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="20">
+        <v>1</v>
+      </c>
+      <c r="J2" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>999</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="21">
+        <v>2</v>
+      </c>
+      <c r="J3" s="18">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="21">
+        <v>3</v>
+      </c>
+      <c r="J4" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="20">
+        <v>4</v>
+      </c>
+      <c r="J5" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="20">
+        <v>16</v>
+      </c>
+      <c r="J6" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
+        <v>17</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="21">
+        <v>17</v>
+      </c>
+      <c r="J7" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E07692-251A-4483-93A8-3C46A54B1DC8}">
+  <dimension ref="A1:J23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="20">
+        <v>1</v>
+      </c>
+      <c r="J4" s="18"/>
+    </row>
+    <row r="5" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6">
+        <v>999</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="21">
+        <v>2</v>
+      </c>
+      <c r="J5" s="18"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="21">
+        <v>3</v>
+      </c>
+      <c r="J6" s="18"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="20">
+        <v>4</v>
+      </c>
+      <c r="J7" s="18"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1</v>
+      </c>
+      <c r="I8" s="21">
+        <v>5</v>
+      </c>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0</v>
+      </c>
+      <c r="I9" s="21">
+        <v>6</v>
+      </c>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="20">
+        <v>7</v>
+      </c>
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1</v>
+      </c>
+      <c r="I11" s="21">
+        <v>8</v>
+      </c>
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>9</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1</v>
+      </c>
+      <c r="I12" s="21">
+        <v>9</v>
+      </c>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0</v>
+      </c>
+      <c r="I13" s="20">
+        <v>10</v>
+      </c>
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>11</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1</v>
+      </c>
+      <c r="I14" s="21">
+        <v>11</v>
+      </c>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
+        <v>12</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="21">
+        <v>12</v>
+      </c>
+      <c r="J15" s="18"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>13</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="20">
+        <v>13</v>
+      </c>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>14</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0</v>
+      </c>
+      <c r="I17" s="21">
+        <v>14</v>
+      </c>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="16">
+        <v>15</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0</v>
+      </c>
+      <c r="I18" s="21">
+        <v>15</v>
+      </c>
+      <c r="J18" s="18"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>16</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0</v>
+      </c>
+      <c r="I19" s="20">
+        <v>16</v>
+      </c>
+      <c r="J19" s="18"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="16">
+        <v>17</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" s="21">
+        <v>17</v>
+      </c>
+      <c r="J20" s="18"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I21" s="7"/>
+      <c r="J21" s="18"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D23" s="15"/>
+      <c r="I23" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006F03DE-650E-40DA-8050-F78C318544B4}">
+  <dimension ref="A2:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FAED69-AADC-4639-97DE-8DBBB5A46D8E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D074EF-2FBA-401C-B7F0-766679C3BCF4}">
   <dimension ref="A1:J20"/>
   <sheetViews>
@@ -1286,15 +2730,15 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="6.453125" customWidth="1"/>
-    <col min="9" max="9" width="31.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="6.44140625" customWidth="1"/>
+    <col min="9" max="9" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="12">
         <v>0</v>
       </c>
@@ -1326,7 +2770,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>43</v>
       </c>
@@ -1358,7 +2802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>27</v>
       </c>
@@ -1390,7 +2834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>68</v>
       </c>
@@ -1422,7 +2866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>28</v>
       </c>
@@ -1454,7 +2898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>67</v>
       </c>
@@ -1486,7 +2930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>48</v>
       </c>
@@ -1518,7 +2962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>66</v>
       </c>
@@ -1550,7 +2994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>31</v>
       </c>
@@ -1582,7 +3026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>32</v>
       </c>
@@ -1614,7 +3058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>52</v>
       </c>
@@ -1646,7 +3090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>65</v>
       </c>
@@ -1678,7 +3122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>35</v>
       </c>
@@ -1710,7 +3154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>36</v>
       </c>
@@ -1742,7 +3186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>56</v>
       </c>
@@ -1774,7 +3218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>57</v>
       </c>
@@ -1806,7 +3250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>58</v>
       </c>
@@ -1838,7 +3282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
         <v>38</v>
       </c>
@@ -1870,10 +3314,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I20" s="7"/>
     </row>
   </sheetData>
@@ -1882,7 +3326,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A54980-A8D2-417B-9277-EF7C8A6DDDAA}">
   <dimension ref="A1:I21"/>
   <sheetViews>
@@ -1890,18 +3334,18 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.81640625" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" customWidth="1"/>
+    <col min="1" max="1" width="46.77734375" customWidth="1"/>
+    <col min="9" max="9" width="26.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1928,7 +3372,7 @@
       </c>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>60</v>
       </c>
@@ -1949,7 +3393,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>27</v>
       </c>
@@ -1976,7 +3420,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>39</v>
       </c>
@@ -2005,7 +3449,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
@@ -2030,7 +3474,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>40</v>
       </c>
@@ -2057,7 +3501,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
@@ -2084,7 +3528,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>30</v>
       </c>
@@ -2113,7 +3557,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
@@ -2142,7 +3586,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>32</v>
       </c>
@@ -2169,7 +3613,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>33</v>
       </c>
@@ -2198,7 +3642,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -2227,7 +3671,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>35</v>
       </c>
@@ -2252,7 +3696,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>36</v>
       </c>
@@ -2277,7 +3721,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>41</v>
       </c>
@@ -2302,7 +3746,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>37</v>
       </c>
@@ -2327,7 +3771,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>42</v>
       </c>
@@ -2354,7 +3798,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>38</v>
       </c>
@@ -2377,10 +3821,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I21" s="7"/>
     </row>
   </sheetData>
@@ -2389,7 +3833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77EA910D-577D-4F2A-8A4F-C91FD8989B4B}">
   <dimension ref="A1:I21"/>
   <sheetViews>
@@ -2397,18 +3841,18 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.81640625" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" customWidth="1"/>
+    <col min="1" max="1" width="46.77734375" customWidth="1"/>
+    <col min="9" max="9" width="26.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -2435,7 +3879,7 @@
       </c>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>60</v>
       </c>
@@ -2456,7 +3900,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>27</v>
       </c>
@@ -2483,7 +3927,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>39</v>
       </c>
@@ -2512,7 +3956,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
@@ -2537,7 +3981,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>40</v>
       </c>
@@ -2564,7 +4008,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
@@ -2591,7 +4035,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>30</v>
       </c>
@@ -2620,7 +4064,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
@@ -2649,7 +4093,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>32</v>
       </c>
@@ -2676,7 +4120,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>33</v>
       </c>
@@ -2705,7 +4149,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -2734,7 +4178,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>35</v>
       </c>
@@ -2759,7 +4203,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>36</v>
       </c>
@@ -2784,7 +4228,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>41</v>
       </c>
@@ -2809,7 +4253,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>37</v>
       </c>
@@ -2834,7 +4278,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>42</v>
       </c>
@@ -2861,7 +4305,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>38</v>
       </c>
@@ -2884,10 +4328,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I21" s="7"/>
     </row>
   </sheetData>
@@ -2896,7 +4340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D278AA97-8598-4E54-B5D9-6A2F7B5081A9}">
   <dimension ref="A1:I22"/>
   <sheetViews>
@@ -2904,18 +4348,18 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.81640625" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" customWidth="1"/>
+    <col min="1" max="1" width="46.77734375" customWidth="1"/>
+    <col min="9" max="9" width="26.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -2942,7 +4386,7 @@
       </c>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>60</v>
       </c>
@@ -2963,7 +4407,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -2990,7 +4434,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>39</v>
       </c>
@@ -3019,7 +4463,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>28</v>
       </c>
@@ -3044,7 +4488,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>40</v>
       </c>
@@ -3071,7 +4515,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
@@ -3098,7 +4542,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
@@ -3127,7 +4571,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -3156,7 +4600,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>32</v>
       </c>
@@ -3183,7 +4627,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
@@ -3212,7 +4656,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>34</v>
       </c>
@@ -3241,7 +4685,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
@@ -3266,7 +4710,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
@@ -3291,7 +4735,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>41</v>
       </c>
@@ -3316,7 +4760,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>37</v>
       </c>
@@ -3341,7 +4785,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
@@ -3368,7 +4812,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
@@ -3391,503 +4835,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I22" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>